<commit_message>
Added processing of a table with a list of years allowed for selection.
</commit_message>
<xml_diff>
--- a/Parameters/Years4Periods.xlsx
+++ b/Parameters/Years4Periods.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dim-Dim\MyData\Common Work Place\Projects\DES.LM.Reports - Production\04. Настройки\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dim-Dim\MyData\Common Work Place\Projects\DES.LM.Reports\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3735721B-9729-40BE-9DD3-3F8A285D241B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FEECFB-744E-4867-8334-68AD1711E459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-12045" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Years" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcCompleted="0" calcOnSave="0"/>
+  <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -360,9 +360,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -376,11 +378,16 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2022</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>2023</v>
       </c>
     </row>

</xml_diff>